<commit_message>
add sendback function,remote db
</commit_message>
<xml_diff>
--- a/tools/xlsx2xml/xlsx/LocalServer/LocalServerConfig.xlsx
+++ b/tools/xlsx2xml/xlsx/LocalServer/LocalServerConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20055" windowHeight="7350"/>
+    <workbookView windowWidth="25320" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="LocalServerConfig" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
     <t>DatabaseFile</t>
   </si>
   <si>
-    <t>ServerDB.db</t>
+    <t>LocalServerDB.db</t>
   </si>
   <si>
     <t>DB File Path</t>
@@ -67,8 +67,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -80,6 +80,73 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -88,29 +155,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -123,11 +170,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -139,21 +186,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,22 +196,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -192,27 +209,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -233,37 +233,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,145 +413,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,6 +424,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -451,45 +475,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -506,6 +497,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,10 +532,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -544,133 +544,133 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1000,7 +1000,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
upload,get,create dir auto recursively
</commit_message>
<xml_diff>
--- a/tools/xlsx2xml/xlsx/LocalServer/LocalServerConfig.xlsx
+++ b/tools/xlsx2xml/xlsx/LocalServer/LocalServerConfig.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17">
   <si>
     <t>Key</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>StreamRelayServer Port</t>
+  </si>
+  <si>
+    <t>FileCacheBaseDir</t>
+  </si>
+  <si>
+    <t>D:/DevelopProj/Dadao/DDRFramework/localwww/</t>
   </si>
 </sst>
 </file>
@@ -66,10 +72,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -80,31 +86,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -119,7 +103,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -127,6 +111,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -141,40 +133,32 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -186,16 +170,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -203,22 +224,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,25 +239,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,157 +413,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -452,6 +458,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -468,20 +489,29 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -500,30 +530,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -532,10 +538,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -544,139 +550,142 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -997,16 +1006,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="1" max="1" width="24.125" customWidth="1"/>
+    <col min="2" max="2" width="47.625" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1076,6 +1085,14 @@
         <v>14</v>
       </c>
     </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>